<commit_message>
adding login for manager + db admin
</commit_message>
<xml_diff>
--- a/src/data/dataMeja.xlsx
+++ b/src/data/dataMeja.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITREP\Repo-Kel2\FoodCourt\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\NetBeansProjects\FoodCourt\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -342,9 +342,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1</v>
       </c>
@@ -352,7 +352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
@@ -360,7 +360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -368,7 +368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4</v>
       </c>
@@ -376,7 +376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
@@ -384,7 +384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -392,7 +392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>7</v>
       </c>
@@ -400,7 +400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>8</v>
       </c>
@@ -408,7 +408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
@@ -416,7 +416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>10</v>
       </c>
@@ -424,7 +424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>11</v>
       </c>
@@ -432,7 +432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>12</v>
       </c>
@@ -440,7 +440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>13</v>
       </c>
@@ -448,7 +448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>14</v>
       </c>
@@ -456,7 +456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>15</v>
       </c>
@@ -464,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>16</v>
       </c>
@@ -472,7 +472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>17</v>
       </c>
@@ -480,7 +480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>18</v>
       </c>
@@ -488,7 +488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>19</v>
       </c>
@@ -496,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Edit Form Table: - Re-layouting Edit form MenuUtama: - Gambar diganti
</commit_message>
<xml_diff>
--- a/src/data/dataMeja.xlsx
+++ b/src/data/dataMeja.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\NetBeansProjects\FoodCourt\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Regawa\Documents\NetBeansProjects\PROYEK1\proyek_kel2\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,12 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -339,12 +343,12 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -352,7 +356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -360,7 +364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -368,15 +372,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -384,23 +388,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -408,23 +412,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -432,47 +436,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -480,28 +484,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit Form Pemesanan: - Write ke ecel pemesanan dari meja
</commit_message>
<xml_diff>
--- a/src/data/dataMeja.xlsx
+++ b/src/data/dataMeja.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Regawa\Documents\NetBeansProjects\PROYEK1\proyek_kel2\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7680"/>
+    <workbookView windowHeight="7680" windowWidth="15330" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,11 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -56,16 +57,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -82,10 +83,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -120,7 +121,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -155,7 +156,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,21 +250,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -280,7 +281,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -332,15 +333,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -352,48 +353,48 @@
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>0</v>
+      <c r="B1" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -509,6 +510,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>